<commit_message>
Add results for random forest
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbw5/Development/github/acc471-final-report/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmusil/Development/acc471-final-report/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35260" yWindow="-640" windowWidth="26740" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="11660" yWindow="460" windowWidth="26740" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data-dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -35,25 +35,16 @@
     <t>Values</t>
   </si>
   <si>
-    <t>Keep</t>
-  </si>
-  <si>
     <t>symboling</t>
   </si>
   <si>
     <t>-3, -2, -1, 0, 1, 2, 3</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>normalized-losses</t>
   </si>
   <si>
     <t>continuous from [65 to 256]</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>make</t>
@@ -515,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,9 +518,9 @@
     <col min="3" max="3" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -537,372 +528,291 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>